<commit_message>
Aanpassingen om ook ontbrekende velden mogelijk te maken in de geproduceerde UNION view
</commit_message>
<xml_diff>
--- a/data_import/basiskaart/tests/fixtures/views/20170216_wms_kaart_database.xlsx
+++ b/data_import/basiskaart/tests/fixtures/views/20170216_wms_kaart_database.xlsx
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Blad1!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t xml:space="preserve">SCHEMA/SERVICE</t>
   </si>
@@ -77,6 +78,24 @@
   </si>
   <si>
     <t xml:space="preserve">BGT_SPR_trein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGT_OBW_opslagtank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gebouw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vlak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lokaalid, bgttype, plustype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGT_OBW_overkapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGT_PND_pand</t>
   </si>
 </sst>
 </file>
@@ -344,27 +363,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -499,6 +518,108 @@
       </c>
       <c r="J4" s="7" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f aca="false">CONCATENATE(C5,"_",D5,"&lt;hoogteligging&gt;")</f>
+        <v>gebouw_vlak&lt;hoogteligging&gt;</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="str">
+        <f aca="false">C5</f>
+        <v>gebouw</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <f aca="false">CONCATENATE(C6,"_",D6,"&lt;hoogteligging&gt;")</f>
+        <v>gebouw_vlak&lt;hoogteligging&gt;</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="str">
+        <f aca="false">C6</f>
+        <v>gebouw</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f aca="false">CONCATENATE(C7,"_",D7,"&lt;hoogteligging&gt;")</f>
+        <v>gebouw_vlak&lt;hoogteligging&gt;</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="5" t="str">
+        <f aca="false">C7</f>
+        <v>gebouw</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +648,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -553,7 +674,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>